<commit_message>
updated strain names and experiment conditions
</commit_message>
<xml_diff>
--- a/old_database/crypto/bioSample/bioSample_1573.xlsx
+++ b/old_database/crypto/bioSample/bioSample_1573.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/old_database/crypto/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF9B0EA-29FD-4142-8D2C-73748143F4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="15640" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="29">
   <si>
     <t>harvestDate</t>
   </si>
@@ -55,9 +61,6 @@
     <t>05.12.15</t>
   </si>
   <si>
-    <t>Retrofitted_1573</t>
-  </si>
-  <si>
     <t>CNAG_00000</t>
   </si>
   <si>
@@ -80,13 +83,37 @@
   </si>
   <si>
     <t>37C.CO2</t>
+  </si>
+  <si>
+    <t>90minuteInduction</t>
+  </si>
+  <si>
+    <t>S.GISH</t>
+  </si>
+  <si>
+    <t>KN99alpha</t>
+  </si>
+  <si>
+    <t>TDY1452</t>
+  </si>
+  <si>
+    <t>TDY1118</t>
+  </si>
+  <si>
+    <t>TDY1451</t>
+  </si>
+  <si>
+    <t>TDY1665</t>
+  </si>
+  <si>
+    <t>TDY1652</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +176,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -195,7 +230,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,9 +262,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -261,6 +314,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -436,14 +507,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,21 +554,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>90</v>
@@ -504,21 +583,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K3">
         <v>90</v>
@@ -527,21 +612,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4">
         <v>90</v>
@@ -550,21 +641,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K5">
         <v>90</v>
@@ -573,21 +670,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6">
         <v>90</v>
@@ -596,21 +699,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>90</v>
@@ -619,21 +728,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8">
         <v>90</v>
@@ -642,21 +757,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>90</v>
@@ -665,21 +786,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10">
         <v>90</v>
@@ -688,21 +815,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11">
         <v>90</v>
@@ -711,21 +844,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K12">
         <v>90</v>
@@ -734,21 +873,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13">
         <v>90</v>
@@ -757,21 +902,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14">
         <v>90</v>
@@ -780,21 +931,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15">
         <v>90</v>
@@ -803,21 +960,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>27</v>
+      </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K16">
         <v>90</v>
@@ -826,21 +989,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
       <c r="G17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K17">
         <v>90</v>
@@ -849,21 +1018,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18">
         <v>90</v>
@@ -872,21 +1047,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
       <c r="G19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19">
         <v>90</v>
@@ -895,21 +1076,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>90</v>
@@ -918,21 +1105,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
       <c r="G21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K21">
         <v>90</v>
@@ -941,21 +1134,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
       <c r="G22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22">
         <v>90</v>

</xml_diff>